<commit_message>
additional analysis on FSR_S2
</commit_message>
<xml_diff>
--- a/data/FSR_S2/stability/FSR_S2 Stability Data.xlsx
+++ b/data/FSR_S2/stability/FSR_S2 Stability Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amro365-my.sharepoint.com/personal/pr19556_appliedmed_com/Documents/Desktop/FSR/data/FSR_S2/stability/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickruiz/Desktop/FSR/data/FSR_S2/stability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{FCD01CB3-A679-4E48-AC6D-BEC61BD358C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF9DB36A-33F3-4B04-B1FB-E7599E50853B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48353EF-D190-5B40-AFD0-51C4C8525954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="2805" windowWidth="21600" windowHeight="12735" xr2:uid="{05FAEE67-03BB-4EED-BB39-2994B23103BF}"/>
+    <workbookView xWindow="-21600" yWindow="-14520" windowWidth="21600" windowHeight="37900" xr2:uid="{05FAEE67-03BB-4EED-BB39-2994B23103BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -166,7 +166,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -272,7 +272,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -414,7 +414,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -424,21 +424,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F91B404-E44C-43FD-8798-D46178A2E488}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -484,7 +484,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -507,7 +507,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>

</xml_diff>